<commit_message>
working solution for call part
</commit_message>
<xml_diff>
--- a/data/cl_planned_schedule.xlsx
+++ b/data/cl_planned_schedule.xlsx
@@ -58,73 +58,73 @@
     <t>weekday1</t>
   </si>
   <si>
+    <t>weekday2</t>
+  </si>
+  <si>
     <t>weekday3</t>
   </si>
   <si>
+    <t>weekend7</t>
+  </si>
+  <si>
+    <t>weekend10</t>
+  </si>
+  <si>
+    <t>weekend11</t>
+  </si>
+  <si>
+    <t>weekend1</t>
+  </si>
+  <si>
+    <t>weekend2</t>
+  </si>
+  <si>
+    <t>weekday4</t>
+  </si>
+  <si>
+    <t>weekday8</t>
+  </si>
+  <si>
+    <t>weekday9</t>
+  </si>
+  <si>
+    <t>weekend13</t>
+  </si>
+  <si>
+    <t>weekend4</t>
+  </si>
+  <si>
+    <t>weekend5</t>
+  </si>
+  <si>
+    <t>weekend8</t>
+  </si>
+  <si>
+    <t>weekend9</t>
+  </si>
+  <si>
+    <t>weekday11</t>
+  </si>
+  <si>
+    <t>weekday12</t>
+  </si>
+  <si>
+    <t>weekday0</t>
+  </si>
+  <si>
+    <t>weekend3</t>
+  </si>
+  <si>
     <t>weekday5</t>
   </si>
   <si>
-    <t>weekend10</t>
-  </si>
-  <si>
-    <t>weekend11</t>
-  </si>
-  <si>
-    <t>weekend1</t>
-  </si>
-  <si>
-    <t>weekend4</t>
-  </si>
-  <si>
-    <t>weekend5</t>
-  </si>
-  <si>
     <t>weekday7</t>
   </si>
   <si>
-    <t>weekday8</t>
-  </si>
-  <si>
-    <t>weekday9</t>
+    <t>weekday10</t>
   </si>
   <si>
     <t>weekend12</t>
-  </si>
-  <si>
-    <t>weekend13</t>
-  </si>
-  <si>
-    <t>weekday2</t>
-  </si>
-  <si>
-    <t>weekend7</t>
-  </si>
-  <si>
-    <t>weekend8</t>
-  </si>
-  <si>
-    <t>weekend9</t>
-  </si>
-  <si>
-    <t>weekday11</t>
-  </si>
-  <si>
-    <t>weekday12</t>
-  </si>
-  <si>
-    <t>weekday0</t>
-  </si>
-  <si>
-    <t>weekend2</t>
-  </si>
-  <si>
-    <t>weekend3</t>
-  </si>
-  <si>
-    <t>weekday4</t>
-  </si>
-  <si>
-    <t>weekday10</t>
   </si>
   <si>
     <t>weekday</t>
@@ -677,19 +677,19 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="2">
-        <v>44760</v>
+        <v>44753</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -698,7 +698,7 @@
         <v>37</v>
       </c>
       <c r="I7">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -706,19 +706,19 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="2">
-        <v>44761</v>
+        <v>44754</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -727,7 +727,7 @@
         <v>37</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -735,19 +735,19 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="2">
-        <v>44762</v>
+        <v>44755</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -756,7 +756,7 @@
         <v>37</v>
       </c>
       <c r="I9">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -764,19 +764,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="2">
-        <v>44763</v>
+        <v>44756</v>
       </c>
       <c r="G10">
         <v>5</v>
@@ -785,7 +785,7 @@
         <v>37</v>
       </c>
       <c r="I10">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -793,19 +793,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="2">
-        <v>44764</v>
+        <v>44757</v>
       </c>
       <c r="G11">
         <v>6</v>
@@ -814,7 +814,7 @@
         <v>37</v>
       </c>
       <c r="I11">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -822,19 +822,19 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="2">
-        <v>44774</v>
+        <v>44760</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -843,7 +843,7 @@
         <v>37</v>
       </c>
       <c r="I12">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -851,19 +851,19 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="2">
-        <v>44775</v>
+        <v>44761</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -872,7 +872,7 @@
         <v>37</v>
       </c>
       <c r="I13">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -880,19 +880,19 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="2">
-        <v>44776</v>
+        <v>44762</v>
       </c>
       <c r="G14">
         <v>4</v>
@@ -901,7 +901,7 @@
         <v>37</v>
       </c>
       <c r="I14">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -909,19 +909,19 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="2">
-        <v>44777</v>
+        <v>44763</v>
       </c>
       <c r="G15">
         <v>5</v>
@@ -930,7 +930,7 @@
         <v>37</v>
       </c>
       <c r="I15">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -938,19 +938,19 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="2">
-        <v>44778</v>
+        <v>44764</v>
       </c>
       <c r="G16">
         <v>6</v>
@@ -959,7 +959,7 @@
         <v>37</v>
       </c>
       <c r="I16">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -967,19 +967,19 @@
         <v>9</v>
       </c>
       <c r="B17">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="2">
-        <v>44800</v>
+        <v>44779</v>
       </c>
       <c r="G17">
         <v>7</v>
@@ -988,7 +988,7 @@
         <v>38</v>
       </c>
       <c r="I17">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -996,19 +996,19 @@
         <v>9</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="2">
-        <v>44801</v>
+        <v>44780</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1017,7 +1017,7 @@
         <v>38</v>
       </c>
       <c r="I18">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1025,19 +1025,19 @@
         <v>9</v>
       </c>
       <c r="B19">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>44807</v>
+        <v>44800</v>
       </c>
       <c r="G19">
         <v>7</v>
@@ -1046,7 +1046,7 @@
         <v>38</v>
       </c>
       <c r="I19">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1054,19 +1054,19 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="2">
-        <v>44808</v>
+        <v>44801</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1075,27 +1075,27 @@
         <v>38</v>
       </c>
       <c r="I20">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="2">
-        <v>44744</v>
+        <v>44807</v>
       </c>
       <c r="G21">
         <v>7</v>
@@ -1104,27 +1104,27 @@
         <v>38</v>
       </c>
       <c r="I21">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="2">
-        <v>44745</v>
+        <v>44808</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1133,7 +1133,7 @@
         <v>38</v>
       </c>
       <c r="I22">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1141,19 +1141,19 @@
         <v>10</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
         <v>19</v>
       </c>
       <c r="F23" s="2">
-        <v>44765</v>
+        <v>44744</v>
       </c>
       <c r="G23">
         <v>7</v>
@@ -1162,7 +1162,7 @@
         <v>38</v>
       </c>
       <c r="I23">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1170,19 +1170,19 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="2">
-        <v>44766</v>
+        <v>44745</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1191,7 +1191,7 @@
         <v>38</v>
       </c>
       <c r="I24">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1199,19 +1199,19 @@
         <v>10</v>
       </c>
       <c r="B25">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
         <v>20</v>
       </c>
       <c r="F25" s="2">
-        <v>44772</v>
+        <v>44751</v>
       </c>
       <c r="G25">
         <v>7</v>
@@ -1220,7 +1220,7 @@
         <v>38</v>
       </c>
       <c r="I25">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1228,19 +1228,19 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
         <v>20</v>
       </c>
       <c r="F26" s="2">
-        <v>44773</v>
+        <v>44752</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1249,7 +1249,7 @@
         <v>38</v>
       </c>
       <c r="I26">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1257,19 +1257,19 @@
         <v>10</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E27" t="s">
         <v>21</v>
       </c>
       <c r="F27" s="2">
-        <v>44781</v>
+        <v>44767</v>
       </c>
       <c r="G27">
         <v>2</v>
@@ -1278,7 +1278,7 @@
         <v>37</v>
       </c>
       <c r="I27">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1286,19 +1286,19 @@
         <v>10</v>
       </c>
       <c r="B28">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E28" t="s">
         <v>21</v>
       </c>
       <c r="F28" s="2">
-        <v>44782</v>
+        <v>44768</v>
       </c>
       <c r="G28">
         <v>3</v>
@@ -1307,7 +1307,7 @@
         <v>37</v>
       </c>
       <c r="I28">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1315,19 +1315,19 @@
         <v>10</v>
       </c>
       <c r="B29">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E29" t="s">
         <v>21</v>
       </c>
       <c r="F29" s="2">
-        <v>44783</v>
+        <v>44769</v>
       </c>
       <c r="G29">
         <v>4</v>
@@ -1336,7 +1336,7 @@
         <v>37</v>
       </c>
       <c r="I29">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1344,19 +1344,19 @@
         <v>10</v>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
         <v>21</v>
       </c>
       <c r="F30" s="2">
-        <v>44784</v>
+        <v>44770</v>
       </c>
       <c r="G30">
         <v>5</v>
@@ -1365,7 +1365,7 @@
         <v>37</v>
       </c>
       <c r="I30">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1373,19 +1373,19 @@
         <v>10</v>
       </c>
       <c r="B31">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E31" t="s">
         <v>21</v>
       </c>
       <c r="F31" s="2">
-        <v>44785</v>
+        <v>44771</v>
       </c>
       <c r="G31">
         <v>6</v>
@@ -1394,7 +1394,7 @@
         <v>37</v>
       </c>
       <c r="I31">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1692,19 +1692,19 @@
         <v>10</v>
       </c>
       <c r="B42">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
         <v>24</v>
       </c>
       <c r="F42" s="2">
-        <v>44814</v>
+        <v>44821</v>
       </c>
       <c r="G42">
         <v>7</v>
@@ -1713,7 +1713,7 @@
         <v>38</v>
       </c>
       <c r="I42">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1721,19 +1721,19 @@
         <v>10</v>
       </c>
       <c r="B43">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E43" t="s">
         <v>24</v>
       </c>
       <c r="F43" s="2">
-        <v>44815</v>
+        <v>44822</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -1742,27 +1742,27 @@
         <v>38</v>
       </c>
       <c r="I43">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B44">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
         <v>25</v>
       </c>
       <c r="F44" s="2">
-        <v>44821</v>
+        <v>44765</v>
       </c>
       <c r="G44">
         <v>7</v>
@@ -1771,27 +1771,27 @@
         <v>38</v>
       </c>
       <c r="I44">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B45">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E45" t="s">
         <v>25</v>
       </c>
       <c r="F45" s="2">
-        <v>44822</v>
+        <v>44766</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -1800,7 +1800,7 @@
         <v>38</v>
       </c>
       <c r="I45">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1808,28 +1808,28 @@
         <v>11</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E46" t="s">
         <v>26</v>
       </c>
       <c r="F46" s="2">
-        <v>44753</v>
+        <v>44772</v>
       </c>
       <c r="G46">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I46">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1837,28 +1837,28 @@
         <v>11</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E47" t="s">
         <v>26</v>
       </c>
       <c r="F47" s="2">
-        <v>44754</v>
+        <v>44773</v>
       </c>
       <c r="G47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I47">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1866,28 +1866,28 @@
         <v>11</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F48" s="2">
-        <v>44755</v>
+        <v>44786</v>
       </c>
       <c r="G48">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I48">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1895,28 +1895,28 @@
         <v>11</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E49" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F49" s="2">
-        <v>44756</v>
+        <v>44787</v>
       </c>
       <c r="G49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I49">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1924,28 +1924,28 @@
         <v>11</v>
       </c>
       <c r="B50">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E50" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F50" s="2">
-        <v>44757</v>
+        <v>44793</v>
       </c>
       <c r="G50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I50">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1953,28 +1953,28 @@
         <v>11</v>
       </c>
       <c r="B51">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E51" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F51" s="2">
-        <v>44779</v>
+        <v>44794</v>
       </c>
       <c r="G51">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H51" t="s">
         <v>38</v>
       </c>
       <c r="I51">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1982,28 +1982,28 @@
         <v>11</v>
       </c>
       <c r="B52">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F52" s="2">
-        <v>44780</v>
+        <v>44809</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I52">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2011,28 +2011,28 @@
         <v>11</v>
       </c>
       <c r="B53">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E53" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F53" s="2">
-        <v>44786</v>
+        <v>44810</v>
       </c>
       <c r="G53">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I53">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2040,28 +2040,28 @@
         <v>11</v>
       </c>
       <c r="B54">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E54" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F54" s="2">
-        <v>44787</v>
+        <v>44811</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I54">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2069,28 +2069,28 @@
         <v>11</v>
       </c>
       <c r="B55">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E55" t="s">
         <v>29</v>
       </c>
       <c r="F55" s="2">
-        <v>44793</v>
+        <v>44812</v>
       </c>
       <c r="G55">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I55">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2098,28 +2098,28 @@
         <v>11</v>
       </c>
       <c r="B56">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E56" t="s">
         <v>29</v>
       </c>
       <c r="F56" s="2">
-        <v>44794</v>
+        <v>44813</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I56">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2127,19 +2127,19 @@
         <v>11</v>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E57" t="s">
         <v>30</v>
       </c>
       <c r="F57" s="2">
-        <v>44809</v>
+        <v>44816</v>
       </c>
       <c r="G57">
         <v>2</v>
@@ -2148,7 +2148,7 @@
         <v>37</v>
       </c>
       <c r="I57">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2156,19 +2156,19 @@
         <v>11</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E58" t="s">
         <v>30</v>
       </c>
       <c r="F58" s="2">
-        <v>44810</v>
+        <v>44817</v>
       </c>
       <c r="G58">
         <v>3</v>
@@ -2177,7 +2177,7 @@
         <v>37</v>
       </c>
       <c r="I58">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2185,19 +2185,19 @@
         <v>11</v>
       </c>
       <c r="B59">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E59" t="s">
         <v>30</v>
       </c>
       <c r="F59" s="2">
-        <v>44811</v>
+        <v>44818</v>
       </c>
       <c r="G59">
         <v>4</v>
@@ -2206,7 +2206,7 @@
         <v>37</v>
       </c>
       <c r="I59">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2214,19 +2214,19 @@
         <v>11</v>
       </c>
       <c r="B60">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E60" t="s">
         <v>30</v>
       </c>
       <c r="F60" s="2">
-        <v>44812</v>
+        <v>44819</v>
       </c>
       <c r="G60">
         <v>5</v>
@@ -2235,7 +2235,7 @@
         <v>37</v>
       </c>
       <c r="I60">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2243,19 +2243,19 @@
         <v>11</v>
       </c>
       <c r="B61">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E61" t="s">
         <v>30</v>
       </c>
       <c r="F61" s="2">
-        <v>44813</v>
+        <v>44820</v>
       </c>
       <c r="G61">
         <v>6</v>
@@ -2264,152 +2264,152 @@
         <v>37</v>
       </c>
       <c r="I61">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B62">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E62" t="s">
         <v>31</v>
       </c>
       <c r="F62" s="2">
-        <v>44816</v>
+        <v>44743</v>
       </c>
       <c r="G62">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H62" t="s">
         <v>37</v>
       </c>
       <c r="I62">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B63">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E63" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F63" s="2">
-        <v>44817</v>
+        <v>44758</v>
       </c>
       <c r="G63">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H63" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I63">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B64">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F64" s="2">
-        <v>44818</v>
+        <v>44759</v>
       </c>
       <c r="G64">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I64">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B65">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E65" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F65" s="2">
-        <v>44819</v>
+        <v>44774</v>
       </c>
       <c r="G65">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H65" t="s">
         <v>37</v>
       </c>
       <c r="I65">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B66">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E66" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F66" s="2">
-        <v>44820</v>
+        <v>44775</v>
       </c>
       <c r="G66">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H66" t="s">
         <v>37</v>
       </c>
       <c r="I66">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2417,28 +2417,28 @@
         <v>12</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E67" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67" s="2">
+        <v>44776</v>
+      </c>
+      <c r="G67">
+        <v>4</v>
+      </c>
+      <c r="H67" t="s">
+        <v>37</v>
+      </c>
+      <c r="I67">
         <v>32</v>
-      </c>
-      <c r="F67" s="2">
-        <v>44743</v>
-      </c>
-      <c r="G67">
-        <v>6</v>
-      </c>
-      <c r="H67" t="s">
-        <v>37</v>
-      </c>
-      <c r="I67">
-        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2446,28 +2446,28 @@
         <v>12</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E68" t="s">
         <v>33</v>
       </c>
       <c r="F68" s="2">
-        <v>44751</v>
+        <v>44777</v>
       </c>
       <c r="G68">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I68">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2475,28 +2475,28 @@
         <v>12</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E69" t="s">
         <v>33</v>
       </c>
       <c r="F69" s="2">
-        <v>44752</v>
+        <v>44778</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H69" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I69">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2504,28 +2504,28 @@
         <v>12</v>
       </c>
       <c r="B70">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E70" t="s">
         <v>34</v>
       </c>
       <c r="F70" s="2">
-        <v>44758</v>
+        <v>44781</v>
       </c>
       <c r="G70">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H70" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I70">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2533,28 +2533,28 @@
         <v>12</v>
       </c>
       <c r="B71">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E71" t="s">
         <v>34</v>
       </c>
       <c r="F71" s="2">
-        <v>44759</v>
+        <v>44782</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I71">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2562,28 +2562,28 @@
         <v>12</v>
       </c>
       <c r="B72">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E72" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F72" s="2">
-        <v>44767</v>
+        <v>44783</v>
       </c>
       <c r="G72">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H72" t="s">
         <v>37</v>
       </c>
       <c r="I72">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2591,28 +2591,28 @@
         <v>12</v>
       </c>
       <c r="B73">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F73" s="2">
-        <v>44768</v>
+        <v>44784</v>
       </c>
       <c r="G73">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H73" t="s">
         <v>37</v>
       </c>
       <c r="I73">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2620,28 +2620,28 @@
         <v>12</v>
       </c>
       <c r="B74">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F74" s="2">
-        <v>44769</v>
+        <v>44785</v>
       </c>
       <c r="G74">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H74" t="s">
         <v>37</v>
       </c>
       <c r="I74">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2649,28 +2649,28 @@
         <v>12</v>
       </c>
       <c r="B75">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E75" t="s">
         <v>35</v>
       </c>
       <c r="F75" s="2">
-        <v>44770</v>
+        <v>44802</v>
       </c>
       <c r="G75">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H75" t="s">
         <v>37</v>
       </c>
       <c r="I75">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -2678,28 +2678,28 @@
         <v>12</v>
       </c>
       <c r="B76">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E76" t="s">
         <v>35</v>
       </c>
       <c r="F76" s="2">
-        <v>44771</v>
+        <v>44803</v>
       </c>
       <c r="G76">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H76" t="s">
         <v>37</v>
       </c>
       <c r="I76">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2716,13 +2716,13 @@
         <v>18</v>
       </c>
       <c r="E77" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F77" s="2">
-        <v>44802</v>
+        <v>44804</v>
       </c>
       <c r="G77">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H77" t="s">
         <v>37</v>
@@ -2745,13 +2745,13 @@
         <v>18</v>
       </c>
       <c r="E78" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F78" s="2">
-        <v>44803</v>
+        <v>44805</v>
       </c>
       <c r="G78">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H78" t="s">
         <v>37</v>
@@ -2774,13 +2774,13 @@
         <v>18</v>
       </c>
       <c r="E79" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F79" s="2">
-        <v>44804</v>
+        <v>44806</v>
       </c>
       <c r="G79">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H79" t="s">
         <v>37</v>
@@ -2794,28 +2794,28 @@
         <v>12</v>
       </c>
       <c r="B80">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E80" t="s">
         <v>36</v>
       </c>
       <c r="F80" s="2">
-        <v>44805</v>
+        <v>44814</v>
       </c>
       <c r="G80">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H80" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I80">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -2823,28 +2823,28 @@
         <v>12</v>
       </c>
       <c r="B81">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E81" t="s">
         <v>36</v>
       </c>
       <c r="F81" s="2">
-        <v>44806</v>
+        <v>44815</v>
       </c>
       <c r="G81">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I81">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated additional model for jeopardy
</commit_message>
<xml_diff>
--- a/data/cl_planned_schedule.xlsx
+++ b/data/cl_planned_schedule.xlsx
@@ -55,10 +55,64 @@
     <t>Paul</t>
   </si>
   <si>
+    <t>weekday2</t>
+  </si>
+  <si>
+    <t>weekend5</t>
+  </si>
+  <si>
+    <t>weekday7</t>
+  </si>
+  <si>
+    <t>weekday9</t>
+  </si>
+  <si>
+    <t>weekday11</t>
+  </si>
+  <si>
+    <t>weekend12</t>
+  </si>
+  <si>
+    <t>weekday1</t>
+  </si>
+  <si>
+    <t>weekend3</t>
+  </si>
+  <si>
+    <t>weekday4</t>
+  </si>
+  <si>
+    <t>weekend10</t>
+  </si>
+  <si>
+    <t>weekday10</t>
+  </si>
+  <si>
+    <t>weekend13</t>
+  </si>
+  <si>
     <t>weekday0</t>
   </si>
   <si>
-    <t>weekend5</t>
+    <t>weekend1</t>
+  </si>
+  <si>
+    <t>weekend4</t>
+  </si>
+  <si>
+    <t>weekend7</t>
+  </si>
+  <si>
+    <t>weekend9</t>
+  </si>
+  <si>
+    <t>weekday12</t>
+  </si>
+  <si>
+    <t>weekend2</t>
+  </si>
+  <si>
+    <t>weekday3</t>
   </si>
   <si>
     <t>weekday5</t>
@@ -68,60 +122,6 @@
   </si>
   <si>
     <t>weekday8</t>
-  </si>
-  <si>
-    <t>weekend12</t>
-  </si>
-  <si>
-    <t>weekend3</t>
-  </si>
-  <si>
-    <t>weekday3</t>
-  </si>
-  <si>
-    <t>weekend7</t>
-  </si>
-  <si>
-    <t>weekday9</t>
-  </si>
-  <si>
-    <t>weekend10</t>
-  </si>
-  <si>
-    <t>weekday11</t>
-  </si>
-  <si>
-    <t>weekday1</t>
-  </si>
-  <si>
-    <t>weekend2</t>
-  </si>
-  <si>
-    <t>weekend9</t>
-  </si>
-  <si>
-    <t>weekday10</t>
-  </si>
-  <si>
-    <t>weekday12</t>
-  </si>
-  <si>
-    <t>weekend13</t>
-  </si>
-  <si>
-    <t>weekend1</t>
-  </si>
-  <si>
-    <t>weekday2</t>
-  </si>
-  <si>
-    <t>weekend4</t>
-  </si>
-  <si>
-    <t>weekday4</t>
-  </si>
-  <si>
-    <t>weekday7</t>
   </si>
   <si>
     <t>weekend11</t>
@@ -532,28 +532,28 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="2">
-        <v>44743</v>
+        <v>44753</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H2" t="s">
         <v>37</v>
       </c>
       <c r="I2">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -561,28 +561,28 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2">
-        <v>44772</v>
+        <v>44754</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -590,28 +590,28 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2">
-        <v>44773</v>
+        <v>44755</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -619,28 +619,28 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2">
-        <v>44774</v>
+        <v>44756</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
         <v>37</v>
       </c>
       <c r="I5">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -648,28 +648,28 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2">
-        <v>44775</v>
+        <v>44757</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
         <v>37</v>
       </c>
       <c r="I6">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -677,28 +677,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2">
-        <v>44776</v>
+        <v>44772</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I7">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -706,25 +706,25 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="2">
-        <v>44777</v>
+        <v>44773</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I8">
         <v>32</v>
@@ -735,28 +735,28 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="2">
-        <v>44778</v>
+        <v>44781</v>
       </c>
       <c r="G9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H9" t="s">
         <v>37</v>
       </c>
       <c r="I9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -764,25 +764,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="2">
-        <v>44786</v>
+        <v>44782</v>
       </c>
       <c r="G10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10">
         <v>33</v>
@@ -793,28 +793,28 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2">
-        <v>44787</v>
+        <v>44783</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I11">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -822,28 +822,28 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F12" s="2">
-        <v>44788</v>
+        <v>44784</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H12" t="s">
         <v>37</v>
       </c>
       <c r="I12">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -851,28 +851,28 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F13" s="2">
-        <v>44789</v>
+        <v>44785</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H13" t="s">
         <v>37</v>
       </c>
       <c r="I13">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -880,28 +880,28 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="2">
-        <v>44790</v>
+        <v>44795</v>
       </c>
       <c r="G14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H14" t="s">
         <v>37</v>
       </c>
       <c r="I14">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -909,28 +909,28 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="2">
-        <v>44791</v>
+        <v>44796</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H15" t="s">
         <v>37</v>
       </c>
       <c r="I15">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -938,28 +938,28 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="2">
-        <v>44792</v>
+        <v>44797</v>
       </c>
       <c r="G16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H16" t="s">
         <v>37</v>
       </c>
       <c r="I16">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -967,28 +967,28 @@
         <v>9</v>
       </c>
       <c r="B17">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F17" s="2">
-        <v>44814</v>
+        <v>44798</v>
       </c>
       <c r="G17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I17">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -996,231 +996,231 @@
         <v>9</v>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F18" s="2">
-        <v>44815</v>
+        <v>44799</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I18">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>44758</v>
+        <v>44809</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I19">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F20" s="2">
-        <v>44759</v>
+        <v>44810</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I20">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F21" s="2">
-        <v>44760</v>
+        <v>44811</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H21" t="s">
         <v>37</v>
       </c>
       <c r="I21">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F22" s="2">
-        <v>44761</v>
+        <v>44812</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H22" t="s">
         <v>37</v>
       </c>
       <c r="I22">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G23">
         <v>6</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="2">
-        <v>44762</v>
-      </c>
-      <c r="G23">
-        <v>4</v>
-      </c>
       <c r="H23" t="s">
         <v>37</v>
       </c>
       <c r="I23">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F24" s="2">
-        <v>44763</v>
+        <v>44814</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I24">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F25" s="2">
-        <v>44764</v>
+        <v>44815</v>
       </c>
       <c r="G25">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I25">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1228,28 +1228,28 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F26" s="2">
-        <v>44779</v>
+        <v>44746</v>
       </c>
       <c r="G26">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I26">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1257,28 +1257,28 @@
         <v>10</v>
       </c>
       <c r="B27">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F27" s="2">
-        <v>44780</v>
+        <v>44747</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I27">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1286,28 +1286,28 @@
         <v>10</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F28" s="2">
-        <v>44795</v>
+        <v>44748</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H28" t="s">
         <v>37</v>
       </c>
       <c r="I28">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1315,28 +1315,28 @@
         <v>10</v>
       </c>
       <c r="B29">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F29" s="2">
-        <v>44796</v>
+        <v>44749</v>
       </c>
       <c r="G29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H29" t="s">
         <v>37</v>
       </c>
       <c r="I29">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1344,28 +1344,28 @@
         <v>10</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F30" s="2">
-        <v>44797</v>
+        <v>44750</v>
       </c>
       <c r="G30">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H30" t="s">
         <v>37</v>
       </c>
       <c r="I30">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1373,28 +1373,28 @@
         <v>10</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F31" s="2">
-        <v>44798</v>
+        <v>44758</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I31">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1402,28 +1402,28 @@
         <v>10</v>
       </c>
       <c r="B32">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F32" s="2">
-        <v>44799</v>
+        <v>44759</v>
       </c>
       <c r="G32">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I32">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1431,28 +1431,28 @@
         <v>10</v>
       </c>
       <c r="B33">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F33" s="2">
-        <v>44800</v>
+        <v>44767</v>
       </c>
       <c r="G33">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I33">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1460,28 +1460,28 @@
         <v>10</v>
       </c>
       <c r="B34">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F34" s="2">
-        <v>44801</v>
+        <v>44768</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I34">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1489,28 +1489,28 @@
         <v>10</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F35" s="2">
-        <v>44809</v>
+        <v>44769</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H35" t="s">
         <v>37</v>
       </c>
       <c r="I35">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1518,28 +1518,28 @@
         <v>10</v>
       </c>
       <c r="B36">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F36" s="2">
-        <v>44810</v>
+        <v>44770</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H36" t="s">
         <v>37</v>
       </c>
       <c r="I36">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1547,28 +1547,28 @@
         <v>10</v>
       </c>
       <c r="B37">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F37" s="2">
-        <v>44811</v>
+        <v>44771</v>
       </c>
       <c r="G37">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H37" t="s">
         <v>37</v>
       </c>
       <c r="I37">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1576,28 +1576,28 @@
         <v>10</v>
       </c>
       <c r="B38">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F38" s="2">
-        <v>44812</v>
+        <v>44800</v>
       </c>
       <c r="G38">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I38">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1605,48 +1605,48 @@
         <v>10</v>
       </c>
       <c r="B39">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F39" s="2">
-        <v>44813</v>
+        <v>44801</v>
       </c>
       <c r="G39">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I39">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E40" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F40" s="2">
-        <v>44746</v>
+        <v>44802</v>
       </c>
       <c r="G40">
         <v>2</v>
@@ -1655,27 +1655,27 @@
         <v>37</v>
       </c>
       <c r="I40">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F41" s="2">
-        <v>44747</v>
+        <v>44803</v>
       </c>
       <c r="G41">
         <v>3</v>
@@ -1684,27 +1684,27 @@
         <v>37</v>
       </c>
       <c r="I41">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F42" s="2">
-        <v>44748</v>
+        <v>44804</v>
       </c>
       <c r="G42">
         <v>4</v>
@@ -1713,27 +1713,27 @@
         <v>37</v>
       </c>
       <c r="I42">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E43" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F43" s="2">
-        <v>44749</v>
+        <v>44805</v>
       </c>
       <c r="G43">
         <v>5</v>
@@ -1742,27 +1742,27 @@
         <v>37</v>
       </c>
       <c r="I43">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F44" s="2">
-        <v>44750</v>
+        <v>44806</v>
       </c>
       <c r="G44">
         <v>6</v>
@@ -1771,27 +1771,27 @@
         <v>37</v>
       </c>
       <c r="I44">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F45" s="2">
-        <v>44751</v>
+        <v>44821</v>
       </c>
       <c r="G45">
         <v>7</v>
@@ -1800,27 +1800,27 @@
         <v>38</v>
       </c>
       <c r="I45">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E46" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F46" s="2">
-        <v>44752</v>
+        <v>44822</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -1829,7 +1829,7 @@
         <v>38</v>
       </c>
       <c r="I46">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1837,28 +1837,28 @@
         <v>11</v>
       </c>
       <c r="B47">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" s="2">
+        <v>44743</v>
+      </c>
+      <c r="G47">
+        <v>6</v>
+      </c>
+      <c r="H47" t="s">
+        <v>37</v>
+      </c>
+      <c r="I47">
         <v>27</v>
-      </c>
-      <c r="F47" s="2">
-        <v>44793</v>
-      </c>
-      <c r="G47">
-        <v>7</v>
-      </c>
-      <c r="H47" t="s">
-        <v>38</v>
-      </c>
-      <c r="I47">
-        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1866,28 +1866,28 @@
         <v>11</v>
       </c>
       <c r="B48">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="2">
+        <v>44744</v>
+      </c>
+      <c r="G48">
+        <v>7</v>
+      </c>
+      <c r="H48" t="s">
+        <v>38</v>
+      </c>
+      <c r="I48">
         <v>27</v>
-      </c>
-      <c r="F48" s="2">
-        <v>44794</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48" t="s">
-        <v>38</v>
-      </c>
-      <c r="I48">
-        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1895,28 +1895,28 @@
         <v>11</v>
       </c>
       <c r="B49">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="2">
+        <v>44745</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>38</v>
+      </c>
+      <c r="I49">
         <v>28</v>
-      </c>
-      <c r="F49" s="2">
-        <v>44802</v>
-      </c>
-      <c r="G49">
-        <v>2</v>
-      </c>
-      <c r="H49" t="s">
-        <v>37</v>
-      </c>
-      <c r="I49">
-        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1924,28 +1924,28 @@
         <v>11</v>
       </c>
       <c r="B50">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F50" s="2">
-        <v>44803</v>
+        <v>44765</v>
       </c>
       <c r="G50">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I50">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1953,28 +1953,28 @@
         <v>11</v>
       </c>
       <c r="B51">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F51" s="2">
-        <v>44804</v>
+        <v>44766</v>
       </c>
       <c r="G51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I51">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1982,28 +1982,28 @@
         <v>11</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E52" t="s">
         <v>28</v>
       </c>
       <c r="F52" s="2">
-        <v>44805</v>
+        <v>44779</v>
       </c>
       <c r="G52">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I52">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2011,28 +2011,28 @@
         <v>11</v>
       </c>
       <c r="B53">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E53" t="s">
         <v>28</v>
       </c>
       <c r="F53" s="2">
-        <v>44806</v>
+        <v>44780</v>
       </c>
       <c r="G53">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I53">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2040,28 +2040,28 @@
         <v>11</v>
       </c>
       <c r="B54">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E54" t="s">
         <v>29</v>
       </c>
       <c r="F54" s="2">
-        <v>44816</v>
+        <v>44793</v>
       </c>
       <c r="G54">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H54" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I54">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2069,28 +2069,28 @@
         <v>11</v>
       </c>
       <c r="B55">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E55" t="s">
         <v>29</v>
       </c>
       <c r="F55" s="2">
-        <v>44817</v>
+        <v>44794</v>
       </c>
       <c r="G55">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I55">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2107,13 +2107,13 @@
         <v>22</v>
       </c>
       <c r="E56" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F56" s="2">
-        <v>44818</v>
+        <v>44816</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H56" t="s">
         <v>37</v>
@@ -2136,13 +2136,13 @@
         <v>22</v>
       </c>
       <c r="E57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F57" s="2">
-        <v>44819</v>
+        <v>44817</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H57" t="s">
         <v>37</v>
@@ -2165,13 +2165,13 @@
         <v>22</v>
       </c>
       <c r="E58" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F58" s="2">
-        <v>44820</v>
+        <v>44818</v>
       </c>
       <c r="G58">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H58" t="s">
         <v>37</v>
@@ -2185,25 +2185,25 @@
         <v>11</v>
       </c>
       <c r="B59">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E59" t="s">
         <v>30</v>
       </c>
       <c r="F59" s="2">
-        <v>44821</v>
+        <v>44819</v>
       </c>
       <c r="G59">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I59">
         <v>38</v>
@@ -2214,28 +2214,28 @@
         <v>11</v>
       </c>
       <c r="B60">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E60" t="s">
         <v>30</v>
       </c>
       <c r="F60" s="2">
-        <v>44822</v>
+        <v>44820</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I60">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2243,19 +2243,19 @@
         <v>12</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E61" t="s">
         <v>31</v>
       </c>
       <c r="F61" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
       <c r="G61">
         <v>7</v>
@@ -2264,7 +2264,7 @@
         <v>38</v>
       </c>
       <c r="I61">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2272,19 +2272,19 @@
         <v>12</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E62" t="s">
         <v>31</v>
       </c>
       <c r="F62" s="2">
-        <v>44745</v>
+        <v>44752</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -2293,7 +2293,7 @@
         <v>38</v>
       </c>
       <c r="I62">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2301,19 +2301,19 @@
         <v>12</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E63" t="s">
         <v>32</v>
       </c>
       <c r="F63" s="2">
-        <v>44753</v>
+        <v>44760</v>
       </c>
       <c r="G63">
         <v>2</v>
@@ -2322,7 +2322,7 @@
         <v>37</v>
       </c>
       <c r="I63">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2330,19 +2330,19 @@
         <v>12</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E64" t="s">
         <v>32</v>
       </c>
       <c r="F64" s="2">
-        <v>44754</v>
+        <v>44761</v>
       </c>
       <c r="G64">
         <v>3</v>
@@ -2351,7 +2351,7 @@
         <v>37</v>
       </c>
       <c r="I64">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2359,19 +2359,19 @@
         <v>12</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E65" t="s">
         <v>32</v>
       </c>
       <c r="F65" s="2">
-        <v>44755</v>
+        <v>44762</v>
       </c>
       <c r="G65">
         <v>4</v>
@@ -2380,7 +2380,7 @@
         <v>37</v>
       </c>
       <c r="I65">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2388,19 +2388,19 @@
         <v>12</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E66" t="s">
         <v>32</v>
       </c>
       <c r="F66" s="2">
-        <v>44756</v>
+        <v>44763</v>
       </c>
       <c r="G66">
         <v>5</v>
@@ -2409,7 +2409,7 @@
         <v>37</v>
       </c>
       <c r="I66">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2417,19 +2417,19 @@
         <v>12</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E67" t="s">
         <v>32</v>
       </c>
       <c r="F67" s="2">
-        <v>44757</v>
+        <v>44764</v>
       </c>
       <c r="G67">
         <v>6</v>
@@ -2438,7 +2438,7 @@
         <v>37</v>
       </c>
       <c r="I67">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2446,28 +2446,28 @@
         <v>12</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E68" t="s">
         <v>33</v>
       </c>
       <c r="F68" s="2">
-        <v>44765</v>
+        <v>44774</v>
       </c>
       <c r="G68">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I68">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2475,28 +2475,28 @@
         <v>12</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E69" t="s">
         <v>33</v>
       </c>
       <c r="F69" s="2">
-        <v>44766</v>
+        <v>44775</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H69" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I69">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2504,28 +2504,28 @@
         <v>12</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E70" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F70" s="2">
-        <v>44767</v>
+        <v>44776</v>
       </c>
       <c r="G70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H70" t="s">
         <v>37</v>
       </c>
       <c r="I70">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2533,28 +2533,28 @@
         <v>12</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E71" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F71" s="2">
-        <v>44768</v>
+        <v>44777</v>
       </c>
       <c r="G71">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H71" t="s">
         <v>37</v>
       </c>
       <c r="I71">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2562,28 +2562,28 @@
         <v>12</v>
       </c>
       <c r="B72">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E72" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F72" s="2">
-        <v>44769</v>
+        <v>44778</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H72" t="s">
         <v>37</v>
       </c>
       <c r="I72">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2591,28 +2591,28 @@
         <v>12</v>
       </c>
       <c r="B73">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E73" t="s">
         <v>34</v>
       </c>
       <c r="F73" s="2">
-        <v>44770</v>
+        <v>44786</v>
       </c>
       <c r="G73">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H73" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I73">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2620,28 +2620,28 @@
         <v>12</v>
       </c>
       <c r="B74">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E74" t="s">
         <v>34</v>
       </c>
       <c r="F74" s="2">
-        <v>44771</v>
+        <v>44787</v>
       </c>
       <c r="G74">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H74" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I74">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2649,19 +2649,19 @@
         <v>12</v>
       </c>
       <c r="B75">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E75" t="s">
         <v>35</v>
       </c>
       <c r="F75" s="2">
-        <v>44781</v>
+        <v>44788</v>
       </c>
       <c r="G75">
         <v>2</v>
@@ -2670,7 +2670,7 @@
         <v>37</v>
       </c>
       <c r="I75">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -2678,19 +2678,19 @@
         <v>12</v>
       </c>
       <c r="B76">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E76" t="s">
         <v>35</v>
       </c>
       <c r="F76" s="2">
-        <v>44782</v>
+        <v>44789</v>
       </c>
       <c r="G76">
         <v>3</v>
@@ -2699,7 +2699,7 @@
         <v>37</v>
       </c>
       <c r="I76">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2707,19 +2707,19 @@
         <v>12</v>
       </c>
       <c r="B77">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E77" t="s">
         <v>35</v>
       </c>
       <c r="F77" s="2">
-        <v>44783</v>
+        <v>44790</v>
       </c>
       <c r="G77">
         <v>4</v>
@@ -2728,7 +2728,7 @@
         <v>37</v>
       </c>
       <c r="I77">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -2736,19 +2736,19 @@
         <v>12</v>
       </c>
       <c r="B78">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E78" t="s">
         <v>35</v>
       </c>
       <c r="F78" s="2">
-        <v>44784</v>
+        <v>44791</v>
       </c>
       <c r="G78">
         <v>5</v>
@@ -2757,7 +2757,7 @@
         <v>37</v>
       </c>
       <c r="I78">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -2765,19 +2765,19 @@
         <v>12</v>
       </c>
       <c r="B79">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E79" t="s">
         <v>35</v>
       </c>
       <c r="F79" s="2">
-        <v>44785</v>
+        <v>44792</v>
       </c>
       <c r="G79">
         <v>6</v>
@@ -2786,7 +2786,7 @@
         <v>37</v>
       </c>
       <c r="I79">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:9">

</xml_diff>